<commit_message>
make common stats report
</commit_message>
<xml_diff>
--- a/templates/stats.xlsx
+++ b/templates/stats.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -28,10 +28,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -42,9 +49,11 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -73,16 +82,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -144,7 +155,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -176,10 +187,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -211,7 +221,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -387,21 +396,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
@@ -413,7 +422,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -424,24 +433,196 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="3" spans="1:9" ht="18.75">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" ht="18.75">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="18.75">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" ht="18.75">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" ht="18.75">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" ht="18.75">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" ht="18.75">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" ht="18.75">
+      <c r="A10" s="5"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" ht="21">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" ht="18.75">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" ht="18.75">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="18.75">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="18.75">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" ht="18.75">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" ht="18.75">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" ht="18.75">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" ht="18.75">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
pro100 as:. Report excel is needed to debug Occurred a rollback by unpacking zip.
</commit_message>
<xml_diff>
--- a/templates/stats.xlsx
+++ b/templates/stats.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,18 +82,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -155,7 +158,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -187,9 +190,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -221,6 +225,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -396,55 +401,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" ht="18.75">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" ht="18.75">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -455,7 +460,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="18.75">
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -470,7 +475,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" ht="18.75">
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -481,7 +486,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="18.75">
+    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -492,7 +497,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" ht="18.75">
+    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -503,7 +508,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="18.75">
+    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -514,8 +519,8 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="18.75">
-      <c r="A10" s="5"/>
+    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="3"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -525,9 +530,9 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="21">
+    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -536,7 +541,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="18.75">
+    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -547,7 +552,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" ht="18.75">
+    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -558,7 +563,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="18.75">
+    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -569,7 +574,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="18.75">
+    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -580,7 +585,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" ht="18.75">
+    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -591,7 +596,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="18.75">
+    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -602,7 +607,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="18.75">
+    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -613,7 +618,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="18.75">
+    <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>

</xml_diff>